<commit_message>
Videos added to repo
</commit_message>
<xml_diff>
--- a/UIP_P01/ExcelData/data/Employee Sample Data.xlsx
+++ b/UIP_P01/ExcelData/data/Employee Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tech\RPA\UIPATH\Portfolio\UIP_P01\ExcelData\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982939BE-65B3-4485-8DC1-DB64A34AF109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B1379B-8AF5-41F8-8A31-A1354A484D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65C14963-D7D9-489F-85DF-B390E3AF6B64}"/>
+    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{65C14963-D7D9-489F-85DF-B390E3AF6B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>

</xml_diff>